<commit_message>
Remove Exception_Screenshots folder. going to add this to gitignore
</commit_message>
<xml_diff>
--- a/AttachmentPerformer/Data/Config.xlsx
+++ b/AttachmentPerformer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\FoleyBrian-Code\UIPath\EmailSummaryPerformer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\JewlzAndTheBoyz-EmailCategorizationBot-P2\AttachmentPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED20D10-4B99-44F8-A93C-DBD3728F2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F4077D-549E-4EC1-ADF9-3F7085274145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="3900" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -563,7 +566,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Test to see if config file was ignored
</commit_message>
<xml_diff>
--- a/AttachmentPerformer/Data/Config.xlsx
+++ b/AttachmentPerformer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\JewlzAndTheBoyz-EmailCategorizationBot-P2\AttachmentPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F4077D-549E-4EC1-ADF9-3F7085274145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6004A8A9-AAF4-4047-8AF0-5F947790E15C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3900" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
 </sst>
 </file>
@@ -498,7 +495,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -566,14 +563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Testing email_categorization config ignore
</commit_message>
<xml_diff>
--- a/AttachmentPerformer/Data/Config.xlsx
+++ b/AttachmentPerformer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\Desktop\JewlzAndTheBoyz-EmailCategorizationBot-P2\AttachmentPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6004A8A9-AAF4-4047-8AF0-5F947790E15C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D876173E-E428-427A-B9DA-8EB3E4C910F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="3540" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4320" yWindow="1785" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -495,7 +495,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>